<commit_message>
Minor adjustment to audit file
</commit_message>
<xml_diff>
--- a/Initial audit.xlsx
+++ b/Initial audit.xlsx
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>